<commit_message>
Apis development commited by Lakshmi
</commit_message>
<xml_diff>
--- a/E-Insurance_Data_Contract.xlsx
+++ b/E-Insurance_Data_Contract.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -214,7 +214,13 @@
     <t>customerNo</t>
   </si>
   <si>
-    <t>age</t>
+    <t>mobileNo</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
@@ -664,7 +670,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -675,10 +681,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A2:D48"/>
+  <dimension ref="A2:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -758,9 +764,15 @@
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4">
@@ -852,7 +864,7 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>16</v>
@@ -864,20 +876,26 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1"/>
@@ -946,10 +964,10 @@
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="10"/>
@@ -993,17 +1011,17 @@
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+    <row r="40" spans="1:4">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1"/>
@@ -1040,6 +1058,12 @@
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>